<commit_message>
avance de Acciones y logros
</commit_message>
<xml_diff>
--- a/MATERIAL/2. Acciones y Logros/Tabla Paritarias Rurales.xlsx
+++ b/MATERIAL/2. Acciones y Logros/Tabla Paritarias Rurales.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandra Zavattaro\Desktop\RESEÑA 2019\ANUARIO 2019_ CONTENIDO\CONTENIDO ANUARIO\2. Acciones y Logros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\eerr\MATERIAL\2. Acciones y Logros\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4210AA0-C9AF-4611-9519-2CD717472FEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$E$13</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -128,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;\ #,##0.00;[Red]\-&quot;$&quot;\ #,##0.00"/>
   </numFmts>
@@ -338,9 +342,21 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -358,18 +374,6 @@
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -650,52 +654,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E8" sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+    <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -705,12 +709,12 @@
       <c r="D3" s="3">
         <v>1033.44</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+    <row r="4" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -720,43 +724,43 @@
       <c r="D4" s="3">
         <v>1075.45</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="13">
         <v>26112.89</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="13">
         <v>1160.57</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+    <row r="6" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
@@ -766,12 +770,12 @@
       <c r="D8" s="4">
         <v>1292.1500000000001</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -781,10 +785,10 @@
       <c r="D9" s="3">
         <v>1329.15</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
@@ -794,10 +798,10 @@
       <c r="D10" s="3">
         <v>1364.39</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
@@ -807,10 +811,10 @@
       <c r="D11" s="3">
         <v>1399.64</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
@@ -820,10 +824,10 @@
       <c r="D12" s="3">
         <v>1434.88</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
@@ -833,7 +837,7 @@
       <c r="D13" s="3">
         <v>1470.12</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -846,6 +850,6 @@
     <mergeCell ref="D5:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>